<commit_message>
group updates, trying to connect
</commit_message>
<xml_diff>
--- a/koalaBaseData.xlsx
+++ b/koalaBaseData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55ABBA27-70B1-4C10-A183-CABEAC62120B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73823E43-4EE8-4D55-A0B9-6685D26E98A4}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -581,12 +581,15 @@
   <dimension ref="A1:AK9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="B6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">

</xml_diff>